<commit_message>
잉여톤 29회 (잉야톤 2회) Stable Diffusion 기술로 생성한 그림을 47번째 스테이지로 추가한다! https://yyt.life/2023/03/11/the-29.html
</commit_message>
<xml_diff>
--- a/Data/StageSequence.xlsx
+++ b/Data/StageSequence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gb/repos/black-android/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gb\repos\black-android\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F1F740-3DD2-8447-A772-27776141DA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B12BA8C-0C16-4933-A121-A2E8963B132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="1260" windowWidth="28100" windowHeight="15920" xr2:uid="{DBF5C1B9-6F6E-44EA-A356-53DB08A15C4F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{DBF5C1B9-6F6E-44EA-A356-53DB08A15C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="161">
   <si>
     <t>[StageSequenceData]</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>MrHup</t>
+  </si>
+  <si>
+    <t>인공 도시</t>
+  </si>
+  <si>
+    <t>인공지능 기술로 그린 그림. 이제 인간이 설 자리는 어디인가?</t>
   </si>
 </sst>
 </file>
@@ -583,7 +595,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -879,30 +891,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEDB4F4-6C8D-4C33-B0CD-FA891662E51F}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -928,7 +940,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -954,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -980,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1032,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1084,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1240,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1263,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1289,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1416,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1442,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1494,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1520,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1546,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1598,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1624,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1647,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1699,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1725,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1751,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1774,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1800,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -1826,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -1878,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -1904,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -1930,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -1956,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -1979,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -2025,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -2048,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -2091,6 +2103,32 @@
         <v>0</v>
       </c>
       <c r="H48" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" s="4">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="4">
+        <v>3</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>